<commit_message>
Latest Update In December
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel/StageCredentials.xlsx
+++ b/src/test/resources/Excel/StageCredentials.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>username</t>
   </si>
@@ -30,9 +30,6 @@
     <t>@Abcd1234</t>
   </si>
   <si>
-    <t>pc.controller1.5</t>
-  </si>
-  <si>
     <t>dec4th.proctor.5</t>
   </si>
   <si>
@@ -48,9 +45,6 @@
     <t>Controller</t>
   </si>
   <si>
-    <t>@Abcd1234#</t>
-  </si>
-  <si>
     <t>ExamName</t>
   </si>
   <si>
@@ -64,19 +58,29 @@
   </si>
   <si>
     <t>Schedule 13 dec</t>
+  </si>
+  <si>
+    <t>controller.ne.5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -99,9 +103,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,7 +411,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -428,52 +433,52 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
         <v>11</v>
-      </c>
-      <c r="E1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>4</v>
+      <c r="A2" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>